<commit_message>
Updated content and also made extensive grammar, clarity, formatting, structure improvements
</commit_message>
<xml_diff>
--- a/help/using/assets/CodeQuality-rules-latest-AMS.xlsx
+++ b/help/using/assets/CodeQuality-rules-latest-AMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/jedelson_adobe_com/Documents/AMS/Pathlight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3EBEEB8B-F071-664F-9C92-01DB5238DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AD697D3-8174-D342-BB66-FD2A0E285433}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{3EBEEB8B-F071-664F-9C92-01DB5238DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50B1A3BB-9993-714B-9069-73DE8F09550A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28080" windowHeight="17500" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28060" windowHeight="17500" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="2" r:id="rId1"/>
@@ -858,9 +858,6 @@
     <t>Product interfaces annotated with @ProviderType should not be implemented by custom code.</t>
   </si>
   <si>
-    <t>BannedPaths</t>
-  </si>
-  <si>
     <t>Customer packages should not install content under /libs</t>
   </si>
   <si>
@@ -1108,6 +1105,9 @@
   </si>
   <si>
     <t>The 'Require all granted' directive should not be used in a VirtualHost Directory section with a root directory-path.</t>
+  </si>
+  <si>
+    <t>BannedPath</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1497,7 @@
   <dimension ref="A1:J154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>360</v>
+      </c>
+      <c r="B35" t="s">
         <v>277</v>
-      </c>
-      <c r="B35" t="s">
-        <v>278</v>
       </c>
       <c r="C35" t="s">
         <v>179</v>
@@ -2607,10 +2607,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>278</v>
+      </c>
+      <c r="B66" t="s">
         <v>279</v>
-      </c>
-      <c r="B66" t="s">
-        <v>280</v>
       </c>
       <c r="C66" t="s">
         <v>179</v>
@@ -2621,10 +2621,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>280</v>
+      </c>
+      <c r="B67" t="s">
         <v>281</v>
-      </c>
-      <c r="B67" t="s">
-        <v>282</v>
       </c>
       <c r="C67" t="s">
         <v>179</v>
@@ -2635,10 +2635,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>282</v>
+      </c>
+      <c r="B68" t="s">
         <v>283</v>
-      </c>
-      <c r="B68" t="s">
-        <v>284</v>
       </c>
       <c r="C68" t="s">
         <v>179</v>
@@ -2649,10 +2649,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>297</v>
+      </c>
+      <c r="B69" t="s">
         <v>298</v>
-      </c>
-      <c r="B69" t="s">
-        <v>299</v>
       </c>
       <c r="C69" t="s">
         <v>179</v>
@@ -3091,10 +3091,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B95" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C95" t="s">
         <v>226</v>
@@ -3103,15 +3103,15 @@
         <v>171</v>
       </c>
       <c r="E95" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B96" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C96" t="s">
         <v>226</v>
@@ -3120,15 +3120,15 @@
         <v>171</v>
       </c>
       <c r="E96" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B97" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C97" t="s">
         <v>226</v>
@@ -3137,15 +3137,15 @@
         <v>171</v>
       </c>
       <c r="E97" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B98" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C98" t="s">
         <v>226</v>
@@ -3154,15 +3154,15 @@
         <v>171</v>
       </c>
       <c r="E98" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B99" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C99" t="s">
         <v>226</v>
@@ -3171,15 +3171,15 @@
         <v>171</v>
       </c>
       <c r="E99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B100" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C100" t="s">
         <v>226</v>
@@ -3188,16 +3188,16 @@
         <v>171</v>
       </c>
       <c r="E100" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B101" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C101" t="s">
         <v>226</v>
@@ -3206,15 +3206,15 @@
         <v>171</v>
       </c>
       <c r="E101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C102" t="s">
         <v>226</v>
@@ -3223,15 +3223,15 @@
         <v>171</v>
       </c>
       <c r="E102" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B103" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C103" t="s">
         <v>226</v>
@@ -3240,15 +3240,15 @@
         <v>171</v>
       </c>
       <c r="E103" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B104" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C104" t="s">
         <v>226</v>
@@ -3257,15 +3257,15 @@
         <v>171</v>
       </c>
       <c r="E104" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B105" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C105" t="s">
         <v>226</v>
@@ -3274,15 +3274,15 @@
         <v>171</v>
       </c>
       <c r="E105" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B106" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C106" t="s">
         <v>226</v>
@@ -3291,15 +3291,15 @@
         <v>171</v>
       </c>
       <c r="E106" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B107" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C107" t="s">
         <v>226</v>
@@ -3308,15 +3308,15 @@
         <v>171</v>
       </c>
       <c r="E107" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B108" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C108" t="s">
         <v>226</v>
@@ -3325,15 +3325,15 @@
         <v>171</v>
       </c>
       <c r="E108" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B109" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C109" t="s">
         <v>226</v>
@@ -3342,15 +3342,15 @@
         <v>171</v>
       </c>
       <c r="E109" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B110" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C110" t="s">
         <v>226</v>
@@ -3359,15 +3359,15 @@
         <v>171</v>
       </c>
       <c r="E110" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B111" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C111" t="s">
         <v>226</v>
@@ -3376,24 +3376,24 @@
         <v>171</v>
       </c>
       <c r="E111" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>340</v>
+      </c>
+      <c r="B112" t="s">
+        <v>349</v>
+      </c>
+      <c r="C112" t="s">
+        <v>226</v>
+      </c>
+      <c r="D112" t="s">
+        <v>171</v>
+      </c>
+      <c r="E112" t="s">
         <v>341</v>
-      </c>
-      <c r="B112" t="s">
-        <v>350</v>
-      </c>
-      <c r="C112" t="s">
-        <v>226</v>
-      </c>
-      <c r="D112" t="s">
-        <v>171</v>
-      </c>
-      <c r="E112" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -3670,10 +3670,10 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B129" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C129" t="s">
         <v>226</v>
@@ -3682,15 +3682,15 @@
         <v>175</v>
       </c>
       <c r="E129" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B130" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C130" t="s">
         <v>226</v>
@@ -3699,15 +3699,15 @@
         <v>175</v>
       </c>
       <c r="E130" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B131" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C131" t="s">
         <v>226</v>
@@ -3716,15 +3716,15 @@
         <v>175</v>
       </c>
       <c r="E131" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C132" t="s">
         <v>226</v>
@@ -3733,15 +3733,15 @@
         <v>175</v>
       </c>
       <c r="E132" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B133" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C133" t="s">
         <v>226</v>
@@ -3750,33 +3750,33 @@
         <v>175</v>
       </c>
       <c r="E133" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>289</v>
+      </c>
+      <c r="B134" t="s">
+        <v>291</v>
+      </c>
+      <c r="C134" t="s">
+        <v>226</v>
+      </c>
+      <c r="D134" t="s">
+        <v>175</v>
+      </c>
+      <c r="E134" t="s">
         <v>290</v>
-      </c>
-      <c r="B134" t="s">
-        <v>292</v>
-      </c>
-      <c r="C134" t="s">
-        <v>226</v>
-      </c>
-      <c r="D134" t="s">
-        <v>175</v>
-      </c>
-      <c r="E134" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>299</v>
+      </c>
+      <c r="B135" t="s">
         <v>300</v>
       </c>
-      <c r="B135" t="s">
-        <v>301</v>
-      </c>
       <c r="C135" t="s">
         <v>226</v>
       </c>
@@ -3784,15 +3784,15 @@
         <v>175</v>
       </c>
       <c r="E135" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B136" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C136" t="s">
         <v>226</v>
@@ -3801,7 +3801,7 @@
         <v>175</v>
       </c>
       <c r="E136" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -3809,10 +3809,10 @@
     </row>
     <row r="137" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B137" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C137" t="s">
         <v>226</v>
@@ -3821,7 +3821,7 @@
         <v>175</v>
       </c>
       <c r="E137" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
@@ -3829,10 +3829,10 @@
     </row>
     <row r="138" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B138" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C138" t="s">
         <v>226</v>
@@ -3841,7 +3841,7 @@
         <v>175</v>
       </c>
       <c r="E138" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
@@ -3849,10 +3849,10 @@
     </row>
     <row r="139" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B139" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C139" t="s">
         <v>226</v>
@@ -3861,7 +3861,7 @@
         <v>175</v>
       </c>
       <c r="E139" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
@@ -3869,10 +3869,10 @@
     </row>
     <row r="140" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B140" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C140" t="s">
         <v>226</v>
@@ -3881,7 +3881,7 @@
         <v>175</v>
       </c>
       <c r="E140" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -3889,10 +3889,10 @@
     </row>
     <row r="141" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B141" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C141" t="s">
         <v>226</v>
@@ -3901,7 +3901,7 @@
         <v>175</v>
       </c>
       <c r="E141" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -3909,10 +3909,10 @@
     </row>
     <row r="142" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B142" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C142" t="s">
         <v>226</v>
@@ -3921,7 +3921,7 @@
         <v>175</v>
       </c>
       <c r="E142" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -3929,10 +3929,10 @@
     </row>
     <row r="143" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B143" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C143" t="s">
         <v>226</v>
@@ -3941,7 +3941,7 @@
         <v>175</v>
       </c>
       <c r="E143" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -3949,10 +3949,10 @@
     </row>
     <row r="144" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B144" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C144" t="s">
         <v>226</v>
@@ -3961,7 +3961,7 @@
         <v>175</v>
       </c>
       <c r="E144" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -3969,10 +3969,10 @@
     </row>
     <row r="145" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B145" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C145" t="s">
         <v>226</v>
@@ -3981,7 +3981,7 @@
         <v>175</v>
       </c>
       <c r="E145" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -3989,10 +3989,10 @@
     </row>
     <row r="146" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C146" t="s">
         <v>226</v>
@@ -4001,7 +4001,7 @@
         <v>175</v>
       </c>
       <c r="E146" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>

</xml_diff>